<commit_message>
finished working on email function. Needs debugger for mistakes
</commit_message>
<xml_diff>
--- a/Code/Registro de Clientes.xlsx
+++ b/Code/Registro de Clientes.xlsx
@@ -19,10 +19,10 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Alana Harris</t>
+    <t>Carla Tavares 39</t>
   </si>
   <si>
-    <t>Elizabeth Poe</t>
+    <t>Christina Kamal 11</t>
   </si>
   <si>
     <t>vcalzadillag@gmail.com</t>
@@ -115,6 +115,7 @@
         <f>HYPERLINK("mailto:fapb88ve@gmail.com","fapb88ve@gmail.com")</f>
         <v>fapb88ve@gmail.com</v>
       </c>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
@@ -123,6 +124,7 @@
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" ht="14.25" customHeight="1"/>
     <row r="5" ht="14.25" customHeight="1"/>

</xml_diff>